<commit_message>
Bibliothek erstellt, Funktioniert alles ausser Bestimmung Winkel
</commit_message>
<xml_diff>
--- a/Carrera-Mapping.xlsx
+++ b/Carrera-Mapping.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bmmli.jl/wolke7/Hochschule/25SS/Projekt EPE-CPS/carrera-map/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9E2E4C4C-341C-E34E-9E89-B783130453E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3343B617-06D9-384D-95E7-00D353C06451}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="280" yWindow="500" windowWidth="28240" windowHeight="16020" activeTab="1" xr2:uid="{A916984E-B641-6449-9A6C-05EB72DB3162}"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
-    <sheet name="test" sheetId="2" r:id="rId2"/>
+    <sheet name="Schienentypen" sheetId="1" r:id="rId1"/>
+    <sheet name="Vorlage zur Erstellung CSV" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="31">
   <si>
     <t>straight_standard</t>
   </si>
@@ -108,18 +108,12 @@
     <t>curve_R4_15_outer_</t>
   </si>
   <si>
-    <t>section_1</t>
-  </si>
-  <si>
     <t>SECTION_START</t>
   </si>
   <si>
     <t>Type</t>
   </si>
   <si>
-    <t>name</t>
-  </si>
-  <si>
     <t>pos_x</t>
   </si>
   <si>
@@ -132,18 +126,26 @@
     <t>SECTION_END</t>
   </si>
   <si>
-    <t>section_2</t>
-  </si>
-  <si>
     <t>anzahl</t>
+  </si>
+  <si>
+    <t>Barcode</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -171,8 +173,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -490,7 +493,7 @@
   <dimension ref="A2:A26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -500,12 +503,12 @@
   <sheetData>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
@@ -624,16 +627,17 @@
       </c>
     </row>
   </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4483C55-B1DA-A940-BA11-F066F03265AC}">
-  <dimension ref="A2:F16"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -641,43 +645,48 @@
     <col min="1" max="1" width="27.33203125" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E2" t="s">
-        <v>28</v>
-      </c>
-      <c r="F2" t="s">
-        <v>29</v>
+        <v>23</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>7</v>
+      </c>
+      <c r="D2">
+        <v>5</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3">
-        <v>7</v>
-      </c>
-      <c r="D3">
-        <v>5</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3">
         <v>0</v>
       </c>
     </row>
@@ -693,7 +702,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -708,42 +717,42 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>0</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11">
+        <v>3</v>
+      </c>
+      <c r="D11">
+        <v>580</v>
+      </c>
+      <c r="E11">
+        <v>720</v>
+      </c>
+      <c r="F11">
         <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>24</v>
-      </c>
-      <c r="B12" t="s">
-        <v>31</v>
-      </c>
-      <c r="C12">
-        <v>3</v>
-      </c>
-      <c r="D12">
-        <v>580</v>
-      </c>
-      <c r="E12">
-        <v>720</v>
-      </c>
-      <c r="F12">
-        <v>30</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
@@ -753,12 +762,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -768,9 +772,9 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{2DAA456D-18DF-0A43-A001-113C6AB1A787}">
           <x14:formula1>
-            <xm:f>Tabelle1!$A$1:$A$26</xm:f>
+            <xm:f>Schienentypen!$A$1:$A$26</xm:f>
           </x14:formula1>
-          <xm:sqref>A3:A29</xm:sqref>
+          <xm:sqref>A2:A15 A16:A542</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>